<commit_message>
dodanie do postaci funkcji dodawania Efektów
Zmiana również przynosi ze sobą naprawienie klasy nowychPlikówTworzenie.java, która teraz prawidłowo tworzy nowe klasy.
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Wrogowie" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Uzbrojenie" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Jednorazówki" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="EfektyBitwy" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Wrogowie" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Uzbrojenie" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Jednorazówki" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="EfektyBitwy" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="90">
   <si>
     <t xml:space="preserve">Nazwa</t>
   </si>
@@ -756,6 +756,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -765,6 +766,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -774,6 +776,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odpornośćUlep </t>
     </r>
@@ -783,6 +786,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= </t>
     </r>
@@ -792,6 +796,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -801,6 +806,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -810,6 +816,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odporność</t>
     </r>
@@ -819,6 +826,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
     </r>
@@ -828,6 +836,7 @@
         <color rgb="FF2AACB8"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5;</t>
     </r>
@@ -839,6 +848,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -848,6 +858,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -857,6 +868,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odpornośćUlep </t>
     </r>
@@ -866,6 +878,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= </t>
     </r>
@@ -875,6 +888,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -884,6 +898,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -893,6 +908,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odporność</t>
     </r>
@@ -902,6 +918,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">;</t>
     </r>
@@ -913,7 +930,16 @@
     <t xml:space="preserve">Niewidzialność</t>
   </si>
   <si>
+    <t xml:space="preserve">postać.unikUlep = 30;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postać.unikUlep = postać.unik;</t>
+  </si>
+  <si>
     <t xml:space="preserve">Trucizna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postać.życie-=2;</t>
   </si>
 </sst>
 </file>
@@ -924,7 +950,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1055,24 +1081,6 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC77DBB"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFBCBEC4"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2AACB8"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1116,7 +1124,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1189,15 +1197,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1273,8 +1273,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1578,7 +1684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1703,7 +1809,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1816,7 +1922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1888,36 +1994,36 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="46.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="17" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="17" width="24.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="17" width="15"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="3" t="s">
         <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -1940,15 +2046,13 @@
       <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="0"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="20"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="17" t="s">
         <v>84</v>
       </c>
@@ -1957,22 +2061,23 @@
       <c r="A3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="B3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>87</v>
+      </c>
       <c r="H3" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
+        <v>88</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>89</v>
+      </c>
       <c r="H4" s="17" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
dodanie przedmiotu wykorzystującego Efekty
wymaga dalszej pracy
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId3"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="94">
   <si>
     <t xml:space="preserve">Nazwa</t>
   </si>
@@ -723,6 +723,47 @@
         <charset val="238"/>
       </rPr>
       <t xml:space="preserve">otrzymajObrażenia(zadaneObrażenia);</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">trutka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trutka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int naIle = 3;</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">wrogowie.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">get(cel).dodajEfekt(naIle)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">;</t>
     </r>
   </si>
   <si>
@@ -1926,10 +1967,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1980,6 +2021,20 @@
       </c>
       <c r="D3" s="16" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2000,7 +2055,7 @@
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -2021,65 +2076,65 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="17" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Efekty na siebie się nakładają
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Wrogowie" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Uzbrojenie" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Jednorazówki" sheetId="4" state="visible" r:id="rId6"/>
-    <sheet name="EfektyBitwy" sheetId="5" state="visible" r:id="rId7"/>
+    <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Wrogowie" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Uzbrojenie" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Jednorazówki" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="EfektyBitwy" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -753,7 +753,7 @@
         <family val="3"/>
         <charset val="238"/>
       </rPr>
-      <t xml:space="preserve">get(cel).dodajEfekt(naIle)</t>
+      <t xml:space="preserve">get(cel).dodajEfekt(new Trucizna(gp),naIle)</t>
     </r>
     <r>
       <rPr>
@@ -1314,114 +1314,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1725,7 +1619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1735,7 +1629,7 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="18.24"/>
@@ -1850,7 +1744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1860,7 +1754,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.93"/>
@@ -1963,20 +1857,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="18.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="74.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="53.48"/>
   </cols>
@@ -2023,7 +1917,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>74</v>
       </c>
@@ -2049,19 +1943,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="46.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="10.33"/>

</xml_diff>

<commit_message>
naprawa działania otrzymywania i zadawania obrażeń
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
   <si>
     <t xml:space="preserve">Nazwa</t>
   </si>
@@ -980,6 +980,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -989,6 +990,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -998,6 +1000,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odpornośćUlep </t>
     </r>
@@ -1007,6 +1010,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= </t>
     </r>
@@ -1016,6 +1020,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -1025,6 +1030,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -1034,6 +1040,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odporność</t>
     </r>
@@ -1043,6 +1050,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+</t>
     </r>
@@ -1052,6 +1060,7 @@
         <color rgb="FF2AACB8"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -1061,6 +1070,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">;
 </t>
@@ -1071,6 +1081,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -1080,6 +1091,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -1089,6 +1101,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">unikUlep </t>
     </r>
@@ -1098,6 +1111,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= </t>
     </r>
@@ -1107,6 +1121,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -1116,6 +1131,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -1125,6 +1141,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">unik </t>
     </r>
@@ -1134,6 +1151,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+ </t>
     </r>
@@ -1143,6 +1161,7 @@
         <color rgb="FF2AACB8"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -1152,6 +1171,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">;</t>
     </r>
@@ -1163,6 +1183,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -1172,6 +1193,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -1181,6 +1203,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odpornośćUlep </t>
     </r>
@@ -1190,6 +1213,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= </t>
     </r>
@@ -1199,6 +1223,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -1208,6 +1233,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -1217,6 +1243,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">odporność</t>
     </r>
@@ -1226,6 +1253,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">;
 </t>
@@ -1236,6 +1264,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -1245,6 +1274,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -1254,6 +1284,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">unikUlep </t>
     </r>
@@ -1263,6 +1294,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">= </t>
     </r>
@@ -1272,6 +1304,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">postać</t>
     </r>
@@ -1281,6 +1314,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
     </r>
@@ -1290,6 +1324,7 @@
         <color rgb="FFC77DBB"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">unik</t>
     </r>
@@ -1299,6 +1334,7 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">;</t>
     </r>
@@ -1330,7 +1366,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1461,24 +1497,6 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFC77DBB"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFBCBEC4"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF2AACB8"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1603,7 +1621,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1690,8 +1708,8 @@
   </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1839,8 +1857,8 @@
       <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1" t="n">
-        <v>5</v>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>35</v>
@@ -1998,7 +2016,7 @@
       <selection pane="topLeft" activeCell="G68" activeCellId="0" sqref="G68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="18.24"/>
@@ -2123,7 +2141,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.93"/>
@@ -2236,7 +2254,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.19"/>
@@ -2318,11 +2336,11 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>

</xml_diff>

<commit_message>
stworzenie prostego przejścia z MenuGłówne do MenuWalki
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="104">
   <si>
     <t xml:space="preserve">Nazwa</t>
   </si>
@@ -210,6 +210,24 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">menuWalki</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
@@ -277,6 +295,21 @@
     <t xml:space="preserve">Łotr</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
     <t xml:space="preserve">BROŃ_LEKKA</t>
   </si>
   <si>
@@ -293,6 +326,9 @@
   </si>
   <si>
     <t xml:space="preserve">Boski Sędzia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoskiSędzia</t>
   </si>
   <si>
     <t xml:space="preserve">Bagiennik</t>
@@ -1366,7 +1402,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1431,6 +1467,18 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC77DBB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <i val="true"/>
@@ -1573,11 +1621,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1585,19 +1633,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1605,7 +1653,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1708,8 +1756,8 @@
   </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1835,7 +1883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -1907,17 +1955,41 @@
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K3" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>39</v>
@@ -1925,16 +1997,30 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
+      <c r="S3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="F4" s="4"/>
       <c r="K4" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>38</v>
@@ -1947,12 +2033,26 @@
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
+      <c r="S4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="F5" s="4"/>
       <c r="K5" s="8" t="s">
@@ -1965,17 +2065,43 @@
         <v>37</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O5" s="4"/>
+      <c r="S5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="F6" s="4"/>
+      <c r="S6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="4"/>
@@ -2016,7 +2142,7 @@
       <selection pane="topLeft" activeCell="G68" activeCellId="0" sqref="G68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="18.24"/>
@@ -2063,7 +2189,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>7</v>
@@ -2092,7 +2218,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>5</v>
@@ -2141,7 +2267,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.93"/>
@@ -2152,16 +2278,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2304,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,7 +2321,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,7 +2338,7 @@
         <v>-1</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,7 +2355,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2254,7 +2380,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.19"/>
@@ -2264,58 +2390,58 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2340,7 +2466,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>
@@ -2357,83 +2483,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="17" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="17" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
małe zmiany w arkuszu Danych
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="104">
   <si>
     <t xml:space="preserve">Nazwa</t>
   </si>
@@ -210,6 +210,24 @@
         <color rgb="FFBCBEC4"/>
         <rFont val="JetBrains Mono"/>
         <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFC77DBB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">menuWalki</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.</t>
@@ -277,6 +295,21 @@
     <t xml:space="preserve">Łotr</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
     <t xml:space="preserve">BROŃ_LEKKA</t>
   </si>
   <si>
@@ -293,6 +326,9 @@
   </si>
   <si>
     <t xml:space="preserve">Boski Sędzia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BoskiSędzia</t>
   </si>
   <si>
     <t xml:space="preserve">Bagiennik</t>
@@ -1366,7 +1402,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1431,6 +1467,18 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC77DBB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
     <font>
       <i val="true"/>
@@ -1573,11 +1621,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1585,19 +1633,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1605,7 +1653,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1708,8 +1756,8 @@
   </sheetPr>
   <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1835,7 +1883,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
@@ -1907,17 +1955,41 @@
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="K3" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>39</v>
@@ -1925,16 +1997,40 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
+      <c r="S3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V3" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="F4" s="4"/>
+        <v>54</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="K4" s="8" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>38</v>
@@ -1947,14 +2043,38 @@
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
+      <c r="S4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="F5" s="4"/>
+        <v>56</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="K5" s="8" t="s">
         <v>39</v>
       </c>
@@ -1965,17 +2085,53 @@
         <v>37</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="O5" s="4"/>
+      <c r="S5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V5" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="F6" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="V6" s="12" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="4"/>
@@ -2012,11 +2168,11 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G68" activeCellId="0" sqref="G68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="18.24"/>
@@ -2063,7 +2219,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>7</v>
@@ -2092,7 +2248,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>5</v>
@@ -2141,7 +2297,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.93"/>
@@ -2152,16 +2308,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2334,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2195,7 +2351,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2212,7 +2368,7 @@
         <v>-1</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2229,7 +2385,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2254,7 +2410,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.19"/>
@@ -2264,58 +2420,58 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2340,7 +2496,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>
@@ -2357,83 +2513,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="17" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="17" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodatki graficzne i zmiany w arkuszu danych
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
   <si>
     <t xml:space="preserve">Nazwa</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ognik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Wrogowie/Ognik/ognikd1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/Wrogowie/Ognik/ognikd2.png</t>
   </si>
   <si>
     <t xml:space="preserve">TypUzbrojenia</t>
@@ -2161,11 +2167,11 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="18.24"/>
@@ -2256,10 +2262,10 @@
         <v>10</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>45</v>
+        <v>61</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>44</v>
@@ -2290,7 +2296,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.93"/>
@@ -2301,16 +2307,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2327,7 +2333,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2344,7 +2350,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,7 +2367,7 @@
         <v>-1</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,7 +2384,7 @@
         <v>-1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2403,7 +2409,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.19"/>
@@ -2413,58 +2419,58 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2485,11 +2491,11 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>
@@ -2506,83 +2512,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="G2" s="18"/>
       <c r="H2" s="17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="17" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F5" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
naprawa problemów z rozgrywką
Naprawiłem działanie Uników i Obrony, aby nie występowały często i w dużych wartościach
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId2"/>
@@ -2167,11 +2167,11 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="18.24"/>
@@ -2259,7 +2259,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>61</v>
@@ -2292,11 +2292,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.93"/>
@@ -2327,7 +2327,7 @@
         <v>36</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="4" t="n">
         <v>3</v>
@@ -2344,7 +2344,7 @@
         <v>38</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>3</v>
@@ -2361,7 +2361,7 @@
         <v>37</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>-1</v>
@@ -2378,7 +2378,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4" t="n">
         <v>-1</v>
@@ -2409,7 +2409,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.19"/>
@@ -2495,7 +2495,7 @@
       <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>

</xml_diff>

<commit_message>
przystosowanie programu pod technologię JAR
</commit_message>
<xml_diff>
--- a/zasoby/Dane/Dane.xlsx
+++ b/zasoby/Dane/Dane.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Bohaterowie" sheetId="1" state="visible" r:id="rId2"/>
@@ -2167,11 +2167,11 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="15.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="18.24"/>
@@ -2179,6 +2179,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="4" width="40.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="4" width="33.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="47.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,7 +2255,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="4" t="n">
         <v>7</v>
@@ -2292,11 +2294,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="13.93"/>
@@ -2409,7 +2411,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="18.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.19"/>
@@ -2495,7 +2497,7 @@
       <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="17" width="47.14"/>

</xml_diff>